<commit_message>
Tarting up the labelling
</commit_message>
<xml_diff>
--- a/data/New_Validation_Workbook.xlsx
+++ b/data/New_Validation_Workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="920" windowWidth="33900" windowHeight="23880" activeTab="9"/>
+    <workbookView xWindow="13080" yWindow="920" windowWidth="33900" windowHeight="23880" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name=" Precision &amp; MU" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Std_Add" sheetId="12" r:id="rId9"/>
     <sheet name="XY_Comparison" sheetId="13" r:id="rId10"/>
     <sheet name="Raw Data" sheetId="9" r:id="rId11"/>
+    <sheet name="Key" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Bias!$A$9:$L$288</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="64">
   <si>
     <t>Type</t>
   </si>
@@ -211,6 +212,21 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Analyte</t>
+  </si>
+  <si>
+    <t>Kryptonite</t>
+  </si>
+  <si>
+    <t>Absorbance</t>
   </si>
 </sst>
 </file>
@@ -643,11 +659,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1988380728"/>
-        <c:axId val="-1988377784"/>
+        <c:axId val="-2031524696"/>
+        <c:axId val="-2031535592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1988380728"/>
+        <c:axId val="-2031524696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -656,7 +672,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1988377784"/>
+        <c:crossAx val="-2031535592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -664,7 +680,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1988377784"/>
+        <c:axId val="-2031535592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,7 +691,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1988380728"/>
+        <c:crossAx val="-2031524696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -812,11 +828,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1977962408"/>
-        <c:axId val="-1977959624"/>
+        <c:axId val="-2031591240"/>
+        <c:axId val="-2031594840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1977962408"/>
+        <c:axId val="-2031591240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,12 +842,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1977959624"/>
+        <c:crossAx val="-2031594840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1977959624"/>
+        <c:axId val="-2031594840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +858,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1977962408"/>
+        <c:crossAx val="-2031591240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1614,7 +1630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
@@ -1837,6 +1853,58 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Creating a multi curve linearity option
</commit_message>
<xml_diff>
--- a/data/New_Validation_Workbook.xlsx
+++ b/data/New_Validation_Workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="920" windowWidth="33900" windowHeight="23880" activeTab="11"/>
+    <workbookView xWindow="13080" yWindow="920" windowWidth="33900" windowHeight="23880" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name=" Precision &amp; MU" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="68">
   <si>
     <t>Type</t>
   </si>
@@ -228,6 +228,18 @@
   <si>
     <t>Absorbance</t>
   </si>
+  <si>
+    <t>Response_A</t>
+  </si>
+  <si>
+    <t>Response_C</t>
+  </si>
+  <si>
+    <t>Response_B</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
 </sst>
 </file>
 
@@ -348,8 +360,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -468,7 +482,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -482,6 +496,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -495,6 +510,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -659,11 +675,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2031524696"/>
-        <c:axId val="-2031535592"/>
+        <c:axId val="1810362952"/>
+        <c:axId val="1810427048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2031524696"/>
+        <c:axId val="1810362952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,7 +688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2031535592"/>
+        <c:crossAx val="1810427048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -680,7 +696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2031535592"/>
+        <c:axId val="1810427048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,7 +707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2031524696"/>
+        <c:crossAx val="1810362952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -723,6 +739,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -740,7 +757,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Response</c:v>
+                  <c:v>Response_A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -828,11 +845,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2031591240"/>
-        <c:axId val="-2031594840"/>
+        <c:axId val="-1972492168"/>
+        <c:axId val="1810851128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2031591240"/>
+        <c:axId val="-1972492168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,12 +859,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2031594840"/>
+        <c:crossAx val="1810851128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2031594840"/>
+        <c:axId val="1810851128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,13 +875,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2031591240"/>
+        <c:crossAx val="-1972492168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -918,16 +936,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1865,7 +1883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -7436,31 +7454,49 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>10</v>
       </c>
@@ -7468,8 +7504,17 @@
         <f>A3*1.02+2</f>
         <v>12.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>11.5</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>20</v>
       </c>
@@ -7477,8 +7522,17 @@
         <f t="shared" ref="B4:B7" si="0">A4*1.02+2</f>
         <v>22.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>50</v>
       </c>
@@ -7486,8 +7540,17 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <v>54</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>100</v>
       </c>
@@ -7495,14 +7558,32 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>105</v>
+      </c>
+      <c r="E6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>200</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>206</v>
+      </c>
+      <c r="C7">
+        <v>201</v>
+      </c>
+      <c r="D7">
+        <v>210</v>
+      </c>
+      <c r="E7">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>